<commit_message>
Reporting the Project first time
</commit_message>
<xml_diff>
--- a/Dispensing Log/DispensingHeading.xlsx
+++ b/Dispensing Log/DispensingHeading.xlsx
@@ -480,7 +480,9 @@
           <t>B000</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
       <c r="E2" s="2" t="n">
         <v>45830</v>
       </c>
@@ -501,7 +503,9 @@
           <t>B001</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
       <c r="E3" s="2" t="n">
         <v>45830</v>
       </c>
@@ -522,7 +526,9 @@
           <t>B002</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="n">
+        <v>100</v>
+      </c>
       <c r="E4" s="2" t="n">
         <v>45830</v>
       </c>
@@ -543,7 +549,9 @@
           <t>B003</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="n">
+        <v>100</v>
+      </c>
       <c r="E5" s="2" t="n">
         <v>45830</v>
       </c>

</xml_diff>